<commit_message>
Submission file added with everyones contribution
</commit_message>
<xml_diff>
--- a/Submission_Documents/Group15_Contribution_Sheet.xlsx
+++ b/Submission_Documents/Group15_Contribution_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24321"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2111\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manrajsingh/Documents/Adv Software/GIT/Final_Project/group15/Submission_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="308" documentId="8_{3F637283-CEDC-48B8-99C2-47CECA005D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F789C5F1-5423-41B5-BA31-403DDFC294AA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828928EB-8320-8446-A6E8-6E459AD34D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="250">
   <si>
     <t>Resource or Class</t>
   </si>
@@ -790,7 +790,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -942,11 +942,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1470,14 +1465,14 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1835,18 +1830,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
-      <selection activeCell="C246" sqref="C246"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B184" sqref="B184"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="90.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="90.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1857,7 +1853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1868,8 +1864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1877,8 +1872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1886,8 +1880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1895,8 +1888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1904,8 +1896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="2"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1913,8 +1904,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1922,8 +1912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1931,8 +1920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1940,8 +1928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1949,8 +1936,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2"/>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1958,8 +1944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1967,8 +1952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1976,12 +1960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -1992,8 +1971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="2"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
@@ -2001,8 +1979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="2"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
@@ -2010,8 +1987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="2"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
@@ -2019,8 +1995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="2"/>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
@@ -2028,8 +2003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="2"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
         <v>24</v>
       </c>
@@ -2037,8 +2011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="2"/>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B22" s="2" t="s">
         <v>25</v>
       </c>
@@ -2046,8 +2019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="2"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B23" s="2" t="s">
         <v>26</v>
       </c>
@@ -2055,8 +2027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="2"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B24" s="2" t="s">
         <v>27</v>
       </c>
@@ -2064,12 +2035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
@@ -2080,8 +2046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="2"/>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B27" s="2" t="s">
         <v>30</v>
       </c>
@@ -2089,8 +2054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="2"/>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B28" s="2" t="s">
         <v>31</v>
       </c>
@@ -2098,8 +2062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="2"/>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B29" s="2" t="s">
         <v>32</v>
       </c>
@@ -2107,8 +2070,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="2"/>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B30" s="2" t="s">
         <v>33</v>
       </c>
@@ -2116,8 +2078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="2"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B31" s="2" t="s">
         <v>34</v>
       </c>
@@ -2125,8 +2086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="2"/>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B32" s="2" t="s">
         <v>35</v>
       </c>
@@ -2134,8 +2094,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="2"/>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B33" s="2" t="s">
         <v>36</v>
       </c>
@@ -2143,8 +2102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="2"/>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B34" s="2" t="s">
         <v>37</v>
       </c>
@@ -2152,8 +2110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="2"/>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B35" s="2" t="s">
         <v>38</v>
       </c>
@@ -2161,12 +2118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -2177,8 +2129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="2"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B38" s="2" t="s">
         <v>41</v>
       </c>
@@ -2186,8 +2137,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="2"/>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B39" s="2" t="s">
         <v>42</v>
       </c>
@@ -2195,8 +2145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="2"/>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B40" s="2" t="s">
         <v>43</v>
       </c>
@@ -2204,12 +2153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
@@ -2220,8 +2164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="2"/>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B43" s="2" t="s">
         <v>46</v>
       </c>
@@ -2229,8 +2172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="2"/>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B44" s="2" t="s">
         <v>47</v>
       </c>
@@ -2238,8 +2180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="2"/>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B45" s="2" t="s">
         <v>48</v>
       </c>
@@ -2247,8 +2188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="2"/>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B46" s="2" t="s">
         <v>49</v>
       </c>
@@ -2256,8 +2196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="2"/>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B47" s="2" t="s">
         <v>50</v>
       </c>
@@ -2265,8 +2204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="2"/>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B48" s="2" t="s">
         <v>51</v>
       </c>
@@ -2274,12 +2212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
         <v>52</v>
       </c>
@@ -2290,8 +2223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="2"/>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B51" s="2" t="s">
         <v>54</v>
       </c>
@@ -2299,8 +2231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="2"/>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B52" s="2" t="s">
         <v>55</v>
       </c>
@@ -2308,12 +2239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
         <v>56</v>
       </c>
@@ -2324,8 +2250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="2"/>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B55" s="2" t="s">
         <v>58</v>
       </c>
@@ -2333,12 +2258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="3" t="s">
         <v>59</v>
       </c>
@@ -2349,7 +2269,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="6"/>
       <c r="B58" s="7" t="s">
         <v>62</v>
@@ -2358,7 +2278,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="6"/>
       <c r="B59" s="7" t="s">
         <v>63</v>
@@ -2367,7 +2287,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="6"/>
       <c r="B60" s="7" t="s">
         <v>64</v>
@@ -2376,12 +2296,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="6"/>
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="6" t="s">
         <v>65</v>
       </c>
@@ -2392,7 +2312,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="6"/>
       <c r="B63" s="7" t="s">
         <v>67</v>
@@ -2401,7 +2321,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="6"/>
       <c r="B64" s="7" t="s">
         <v>68</v>
@@ -2410,7 +2330,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="6"/>
       <c r="B65" s="7" t="s">
         <v>69</v>
@@ -2419,7 +2339,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" s="6"/>
       <c r="B66" s="7" t="s">
         <v>70</v>
@@ -2428,12 +2348,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="6"/>
       <c r="B67" s="7"/>
       <c r="C67" s="8"/>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" s="6" t="s">
         <v>71</v>
       </c>
@@ -2444,7 +2364,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A69" s="6"/>
       <c r="B69" s="7" t="s">
         <v>73</v>
@@ -2453,12 +2373,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" s="6"/>
       <c r="B70" s="7"/>
       <c r="C70" s="8"/>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" s="6" t="s">
         <v>74</v>
       </c>
@@ -2469,7 +2389,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" s="6"/>
       <c r="B72" s="7" t="s">
         <v>76</v>
@@ -2478,7 +2398,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="25.5">
+    <row r="73" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A73" s="6"/>
       <c r="B73" s="9" t="s">
         <v>77</v>
@@ -2487,7 +2407,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" s="6"/>
       <c r="B74" s="7" t="s">
         <v>78</v>
@@ -2496,7 +2416,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" s="6"/>
       <c r="B75" s="7" t="s">
         <v>79</v>
@@ -2505,7 +2425,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A76" s="6"/>
       <c r="B76" s="7" t="s">
         <v>80</v>
@@ -2514,7 +2434,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A77" s="6"/>
       <c r="B77" s="7" t="s">
         <v>81</v>
@@ -2523,7 +2443,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A78" s="6"/>
       <c r="B78" s="7" t="s">
         <v>82</v>
@@ -2532,7 +2452,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="38.25">
+    <row r="79" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A79" s="6"/>
       <c r="B79" s="9" t="s">
         <v>83</v>
@@ -2541,7 +2461,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A80" s="6"/>
       <c r="B80" s="7" t="s">
         <v>84</v>
@@ -2550,12 +2470,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A81" s="6"/>
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A82" s="6" t="s">
         <v>85</v>
       </c>
@@ -2566,7 +2486,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A83" s="6"/>
       <c r="B83" s="7" t="s">
         <v>87</v>
@@ -2575,7 +2495,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A84" s="6"/>
       <c r="B84" s="7" t="s">
         <v>88</v>
@@ -2584,7 +2504,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A85" s="6"/>
       <c r="B85" s="7" t="s">
         <v>89</v>
@@ -2593,7 +2513,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A86" s="6"/>
       <c r="B86" s="7" t="s">
         <v>90</v>
@@ -2602,12 +2522,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A87" s="6"/>
       <c r="B87" s="7"/>
       <c r="C87" s="8"/>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A88" s="6" t="s">
         <v>91</v>
       </c>
@@ -2618,7 +2538,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A89" s="6"/>
       <c r="B89" s="7" t="s">
         <v>93</v>
@@ -2627,7 +2547,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A90" s="6"/>
       <c r="B90" s="7" t="s">
         <v>94</v>
@@ -2636,7 +2556,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A91" s="6"/>
       <c r="B91" s="7" t="s">
         <v>95</v>
@@ -2645,12 +2565,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A92" s="6"/>
       <c r="B92" s="7"/>
       <c r="C92" s="8"/>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A93" s="6" t="s">
         <v>96</v>
       </c>
@@ -2661,7 +2581,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A94" s="6"/>
       <c r="B94" s="7" t="s">
         <v>93</v>
@@ -2670,7 +2590,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A95" s="6"/>
       <c r="B95" s="7" t="s">
         <v>94</v>
@@ -2679,7 +2599,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A96" s="6"/>
       <c r="B96" s="7" t="s">
         <v>95</v>
@@ -2688,7 +2608,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A97" s="10"/>
       <c r="B97" s="11" t="s">
         <v>97</v>
@@ -2697,1198 +2617,1193 @@
         <v>61</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
-      <c r="A98" s="14"/>
-      <c r="B98" s="14"/>
-      <c r="C98" s="14"/>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" s="14"/>
-      <c r="B99" s="14"/>
-      <c r="C99" s="14"/>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" s="13" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A98" s="13"/>
+      <c r="B98" s="13"/>
+      <c r="C98" s="13"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A99" s="13"/>
+      <c r="B99" s="13"/>
+      <c r="C99" s="13"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A100" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B100" s="14" t="s">
+      <c r="B100" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C100" s="14" t="s">
+      <c r="C100" s="13" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
-      <c r="B101" s="13" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B101" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C101" s="13" t="s">
+      <c r="C101" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
-      <c r="A102" s="13"/>
-      <c r="B102" s="13"/>
-      <c r="C102" s="13"/>
-    </row>
-    <row r="103" spans="1:3" ht="25.5">
-      <c r="A103" s="13" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A102" s="15"/>
+      <c r="B102" s="15"/>
+      <c r="C102" s="15"/>
+    </row>
+    <row r="103" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A103" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B103" s="15" t="s">
+      <c r="B103" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C103" s="13" t="s">
+      <c r="C103" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
-      <c r="B104" s="13" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B104" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C104" s="13" t="s">
+      <c r="C104" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
-      <c r="A105" s="13"/>
-      <c r="B105" s="13" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A105" s="15"/>
+      <c r="B105" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="C105" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
-      <c r="A106" s="13"/>
-      <c r="B106" s="13" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A106" s="15"/>
+      <c r="B106" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C106" s="13" t="s">
+      <c r="C106" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="13"/>
-      <c r="B107" s="13" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A107" s="15"/>
+      <c r="B107" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C107" s="13" t="s">
+      <c r="C107" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="13"/>
-      <c r="B108" s="13" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A108" s="15"/>
+      <c r="B108" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C108" s="13" t="s">
+      <c r="C108" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
-      <c r="A109" s="13"/>
-      <c r="B109" s="13" t="s">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A109" s="15"/>
+      <c r="B109" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C109" s="13" t="s">
+      <c r="C109" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
-      <c r="A110" s="13"/>
-      <c r="B110" s="13" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A110" s="15"/>
+      <c r="B110" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C110" s="13" t="s">
+      <c r="C110" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
-      <c r="A111" s="13"/>
-      <c r="B111" s="13" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A111" s="15"/>
+      <c r="B111" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="C111" s="13" t="s">
+      <c r="C111" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
-      <c r="A112" s="13"/>
-      <c r="B112" s="13" t="s">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A112" s="15"/>
+      <c r="B112" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C112" s="13" t="s">
+      <c r="C112" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
-      <c r="A113" s="13"/>
-      <c r="B113" s="13" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A113" s="15"/>
+      <c r="B113" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C113" s="13" t="s">
+      <c r="C113" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
-      <c r="A114" s="13"/>
-      <c r="B114" s="13" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A114" s="15"/>
+      <c r="B114" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C114" s="13" t="s">
+      <c r="C114" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
-      <c r="A115" s="13"/>
-      <c r="B115" s="13" t="s">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A115" s="15"/>
+      <c r="B115" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="C115" s="13" t="s">
+      <c r="C115" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="13"/>
-      <c r="B116" s="13" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A116" s="15"/>
+      <c r="B116" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C116" s="13" t="s">
+      <c r="C116" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
-      <c r="A117" s="13"/>
-      <c r="B117" s="13"/>
-      <c r="C117" s="13"/>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" s="13" t="s">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A117" s="15"/>
+      <c r="B117" s="15"/>
+      <c r="C117" s="15"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A118" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B118" s="13" t="s">
+      <c r="B118" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C118" s="13" t="s">
+      <c r="C118" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
-      <c r="B119" s="13" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B119" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="C119" s="13" t="s">
+      <c r="C119" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
-      <c r="B120" s="13" t="s">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B120" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C120" s="13" t="s">
+      <c r="C120" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
-      <c r="A122" s="13" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A122" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="B122" s="13" t="s">
+      <c r="B122" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C122" s="13" t="s">
+      <c r="C122" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
-      <c r="A124" s="13" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A124" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B124" s="13" t="s">
+      <c r="B124" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C124" s="13" t="s">
+      <c r="C124" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
-      <c r="B125" s="13" t="s">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B125" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C125" s="13" t="s">
+      <c r="C125" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
-      <c r="A126" s="13"/>
-      <c r="B126" s="13" t="s">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A126" s="15"/>
+      <c r="B126" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C126" s="13" t="s">
+      <c r="C126" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
-      <c r="A127" s="13"/>
-      <c r="B127" s="13" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A127" s="15"/>
+      <c r="B127" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="C127" s="13" t="s">
+      <c r="C127" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
-      <c r="A128" s="13"/>
-      <c r="B128" s="13"/>
-      <c r="C128" s="13"/>
-    </row>
-    <row r="129" spans="1:3">
-      <c r="A129" s="13" t="s">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A128" s="15"/>
+      <c r="B128" s="15"/>
+      <c r="C128" s="15"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A129" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="B129" s="13" t="s">
+      <c r="B129" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="C129" s="13" t="s">
+      <c r="C129" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
-      <c r="A130" s="13"/>
-      <c r="B130" s="13" t="s">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A130" s="15"/>
+      <c r="B130" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="C130" s="13" t="s">
+      <c r="C130" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
-      <c r="A131" s="13"/>
-      <c r="B131" s="13" t="s">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A131" s="15"/>
+      <c r="B131" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="C131" s="13" t="s">
+      <c r="C131" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
-      <c r="A132" s="13"/>
-      <c r="B132" s="13"/>
-      <c r="C132" s="13"/>
-    </row>
-    <row r="133" spans="1:3">
-      <c r="A133" s="13" t="s">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A132" s="15"/>
+      <c r="B132" s="15"/>
+      <c r="C132" s="15"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A133" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B133" s="13" t="s">
+      <c r="B133" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C133" s="13" t="s">
+      <c r="C133" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
-      <c r="B134" s="13" t="s">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B134" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="C134" s="13" t="s">
+      <c r="C134" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
-      <c r="A135" s="13"/>
-      <c r="B135" s="13"/>
-      <c r="C135" s="13"/>
-    </row>
-    <row r="136" spans="1:3">
-      <c r="A136" s="13" t="s">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A135" s="15"/>
+      <c r="B135" s="15"/>
+      <c r="C135" s="15"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A136" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B136" s="13" t="s">
+      <c r="B136" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C136" s="13" t="s">
+      <c r="C136" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
-      <c r="B137" s="13" t="s">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B137" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="C137" s="13" t="s">
+      <c r="C137" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
-      <c r="A138" s="13"/>
-      <c r="B138" s="13"/>
-      <c r="C138" s="13"/>
-    </row>
-    <row r="139" spans="1:3">
-      <c r="A139" s="13" t="s">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A138" s="15"/>
+      <c r="B138" s="15"/>
+      <c r="C138" s="15"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A139" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="B139" s="13" t="s">
+      <c r="B139" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C139" s="13" t="s">
+      <c r="C139" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
-      <c r="A140" s="13"/>
-      <c r="B140" s="13"/>
-      <c r="C140" s="13"/>
-    </row>
-    <row r="141" spans="1:3">
-      <c r="A141" s="13" t="s">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A140" s="15"/>
+      <c r="B140" s="15"/>
+      <c r="C140" s="15"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A141" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="B141" s="13" t="s">
+      <c r="B141" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="C141" s="13" t="s">
+      <c r="C141" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
-      <c r="B142" s="13" t="s">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B142" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="C142" s="13" t="s">
+      <c r="C142" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
-      <c r="A143" s="13"/>
-      <c r="B143" s="13"/>
-      <c r="C143" s="13"/>
-    </row>
-    <row r="144" spans="1:3">
-      <c r="A144" s="13" t="s">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A143" s="15"/>
+      <c r="B143" s="15"/>
+      <c r="C143" s="15"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A144" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="B144" s="13" t="s">
+      <c r="B144" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C144" s="13" t="s">
+      <c r="C144" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
-      <c r="B145" s="13" t="s">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B145" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="C145" s="13" t="s">
+      <c r="C145" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
-      <c r="A146" s="13"/>
-      <c r="B146" s="13"/>
-      <c r="C146" s="13"/>
-    </row>
-    <row r="147" spans="1:3">
-      <c r="A147" s="13" t="s">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A146" s="15"/>
+      <c r="B146" s="15"/>
+      <c r="C146" s="15"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A147" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B147" s="13" t="s">
+      <c r="B147" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C147" s="13" t="s">
+      <c r="C147" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
-      <c r="B148" s="13" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B148" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C148" s="13" t="s">
+      <c r="C148" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
-      <c r="A151" s="16" t="s">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A151" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="B151" s="16" t="s">
+      <c r="B151" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="C151" s="16" t="s">
+      <c r="C151" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
-      <c r="A152" s="16"/>
-      <c r="B152" s="16"/>
-      <c r="C152" s="16"/>
-    </row>
-    <row r="153" spans="1:3">
-      <c r="A153" s="16" t="s">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A152" s="14"/>
+      <c r="B152" s="14"/>
+      <c r="C152" s="14"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A153" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="B153" s="16" t="s">
+      <c r="B153" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="C153" s="16" t="s">
+      <c r="C153" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
-      <c r="A154" s="16"/>
-      <c r="B154" s="16" t="s">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A154" s="14"/>
+      <c r="B154" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="C154" s="16" t="s">
+      <c r="C154" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
-      <c r="A155" s="16"/>
-      <c r="B155" s="16" t="s">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A155" s="14"/>
+      <c r="B155" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="C155" s="16" t="s">
+      <c r="C155" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
-      <c r="A156" s="16"/>
-      <c r="B156" s="16"/>
-      <c r="C156" s="16"/>
-    </row>
-    <row r="157" spans="1:3">
-      <c r="A157" s="16" t="s">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A156" s="14"/>
+      <c r="B156" s="14"/>
+      <c r="C156" s="14"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A157" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="B157" s="16" t="s">
+      <c r="B157" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C157" s="16" t="s">
+      <c r="C157" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
-      <c r="A158" s="16"/>
-      <c r="B158" s="16" t="s">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A158" s="14"/>
+      <c r="B158" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="C158" s="16" t="s">
+      <c r="C158" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
-      <c r="A159" s="16"/>
-      <c r="B159" s="16"/>
-      <c r="C159" s="16"/>
-    </row>
-    <row r="160" spans="1:3">
-      <c r="A160" s="16" t="s">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A159" s="14"/>
+      <c r="B159" s="14"/>
+      <c r="C159" s="14"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A160" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B160" s="16" t="s">
+      <c r="B160" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="C160" s="16" t="s">
+      <c r="C160" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
-      <c r="A161" s="16"/>
-      <c r="B161" s="16"/>
-      <c r="C161" s="16"/>
-    </row>
-    <row r="162" spans="1:3">
-      <c r="A162" s="16" t="s">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A161" s="14"/>
+      <c r="B161" s="14"/>
+      <c r="C161" s="14"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A162" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="B162" s="16" t="s">
+      <c r="B162" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="C162" s="16" t="s">
+      <c r="C162" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
-      <c r="A163" s="16"/>
-      <c r="B163" s="16" t="s">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A163" s="14"/>
+      <c r="B163" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C163" s="16" t="s">
+      <c r="C163" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
-      <c r="A164" s="16"/>
-      <c r="B164" s="16" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A164" s="14"/>
+      <c r="B164" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="C164" s="16" t="s">
+      <c r="C164" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
-      <c r="A165" s="16"/>
-      <c r="B165" s="16"/>
-      <c r="C165" s="16"/>
-    </row>
-    <row r="166" spans="1:3">
-      <c r="A166" s="16" t="s">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A165" s="14"/>
+      <c r="B165" s="14"/>
+      <c r="C165" s="14"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A166" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="B166" s="16" t="s">
+      <c r="B166" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="C166" s="16" t="s">
+      <c r="C166" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
-      <c r="A167" s="16"/>
-      <c r="B167" s="16"/>
-      <c r="C167" s="16"/>
-    </row>
-    <row r="168" spans="1:3">
-      <c r="A168" s="16" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A167" s="14"/>
+      <c r="B167" s="14"/>
+      <c r="C167" s="14"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A168" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="B168" s="16" t="s">
+      <c r="B168" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C168" s="16" t="s">
+      <c r="C168" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
-      <c r="A169" s="16"/>
-      <c r="B169" s="16"/>
-      <c r="C169" s="16"/>
-    </row>
-    <row r="170" spans="1:3">
-      <c r="A170" s="16" t="s">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A169" s="14"/>
+      <c r="B169" s="14"/>
+      <c r="C169" s="14"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A170" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="B170" s="16" t="s">
+      <c r="B170" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="C170" s="16" t="s">
+      <c r="C170" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
-      <c r="A171" s="16"/>
-      <c r="B171" s="16"/>
-      <c r="C171" s="16"/>
-    </row>
-    <row r="172" spans="1:3">
-      <c r="A172" s="16" t="s">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A171" s="14"/>
+      <c r="B171" s="14"/>
+      <c r="C171" s="14"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A172" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B172" s="16" t="s">
+      <c r="B172" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="C172" s="16" t="s">
+      <c r="C172" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
-      <c r="A173" s="16"/>
-      <c r="B173" s="16"/>
-      <c r="C173" s="16"/>
-    </row>
-    <row r="174" spans="1:3">
-      <c r="A174" s="16" t="s">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A173" s="14"/>
+      <c r="B173" s="14"/>
+      <c r="C173" s="14"/>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A174" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="B174" s="16" t="s">
+      <c r="B174" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="C174" s="16" t="s">
+      <c r="C174" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
-      <c r="A175" s="16"/>
-      <c r="B175" s="16"/>
-      <c r="C175" s="16"/>
-    </row>
-    <row r="176" spans="1:3">
-      <c r="A176" s="16" t="s">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A175" s="14"/>
+      <c r="B175" s="14"/>
+      <c r="C175" s="14"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A176" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="B176" s="16" t="s">
+      <c r="B176" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="C176" s="16" t="s">
+      <c r="C176" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
-      <c r="A177" s="16"/>
-      <c r="B177" s="16" t="s">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A177" s="14"/>
+      <c r="B177" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="C177" s="16" t="s">
+      <c r="C177" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
-      <c r="A178" s="16"/>
-      <c r="B178" s="16" t="s">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A178" s="14"/>
+      <c r="B178" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="C178" s="16" t="s">
+      <c r="C178" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
-      <c r="A179" s="16"/>
-      <c r="B179" s="16" t="s">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A179" s="14"/>
+      <c r="B179" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="C179" s="16" t="s">
+      <c r="C179" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
-      <c r="A180" s="16"/>
-      <c r="B180" s="16" t="s">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A180" s="14"/>
+      <c r="B180" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="C180" s="16" t="s">
+      <c r="C180" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
-      <c r="A181" s="16"/>
-      <c r="B181" s="16"/>
-      <c r="C181" s="16"/>
-    </row>
-    <row r="182" spans="1:3">
-      <c r="A182" s="16" t="s">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A181" s="14"/>
+      <c r="B181" s="14"/>
+      <c r="C181" s="14"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A182" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="B182" s="16" t="s">
+      <c r="B182" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="C182" s="16" t="s">
+      <c r="C182" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
-      <c r="A183" s="16"/>
-      <c r="B183" s="16" t="s">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A183" s="14"/>
+      <c r="B183" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="C183" s="16" t="s">
+      <c r="C183" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
-      <c r="A184" s="16"/>
-      <c r="B184" s="16" t="s">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A184" s="14"/>
+      <c r="B184" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="C184" s="16" t="s">
+      <c r="C184" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
-      <c r="A185" s="16"/>
-      <c r="B185" s="16" t="s">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A185" s="14"/>
+      <c r="B185" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C185" s="16" t="s">
+      <c r="C185" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
-      <c r="A186" s="16"/>
-      <c r="B186" s="16" t="s">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A186" s="14"/>
+      <c r="B186" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="C186" s="16" t="s">
+      <c r="C186" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
-      <c r="A187" s="16"/>
-      <c r="B187" s="16" t="s">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A187" s="14"/>
+      <c r="B187" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="C187" s="16" t="s">
+      <c r="C187" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
-      <c r="A188" s="16"/>
-      <c r="B188" s="16"/>
-      <c r="C188" s="16"/>
-    </row>
-    <row r="189" spans="1:3">
-      <c r="A189" s="16" t="s">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A188" s="14"/>
+      <c r="B188" s="14"/>
+      <c r="C188" s="14"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A189" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="B189" s="16" t="s">
+      <c r="B189" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="C189" s="16" t="s">
+      <c r="C189" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
-      <c r="A190" s="16"/>
-      <c r="B190" s="16" t="s">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A190" s="14"/>
+      <c r="B190" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="C190" s="16" t="s">
+      <c r="C190" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
-      <c r="A192" t="s">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A192" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B192" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B193" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C192" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3">
-      <c r="B193" t="s">
+      <c r="C193" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B194" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C193" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3">
-      <c r="B194" t="s">
-        <v>190</v>
-      </c>
-      <c r="C194" t="s">
+      <c r="C194" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A196" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A198" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B199" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B200" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B201" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B202" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B203" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C203" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
-      <c r="A196" t="s">
-        <v>191</v>
-      </c>
-      <c r="C196" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3">
-      <c r="A198" t="s">
-        <v>193</v>
-      </c>
-      <c r="B198" t="s">
-        <v>194</v>
-      </c>
-      <c r="C198" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3">
-      <c r="B199" t="s">
-        <v>195</v>
-      </c>
-      <c r="C199" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3">
-      <c r="B200" t="s">
-        <v>196</v>
-      </c>
-      <c r="C200" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3">
-      <c r="B201" t="s">
-        <v>197</v>
-      </c>
-      <c r="C201" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3">
-      <c r="B202" t="s">
-        <v>198</v>
-      </c>
-      <c r="C202" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3">
-      <c r="B203" t="s">
-        <v>199</v>
-      </c>
-      <c r="C203" t="s">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B204" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B205" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B206" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C206" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="204" spans="1:3">
-      <c r="B204" t="s">
-        <v>200</v>
-      </c>
-      <c r="C204" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3">
-      <c r="B205" t="s">
-        <v>201</v>
-      </c>
-      <c r="C205" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3">
-      <c r="B206" t="s">
-        <v>189</v>
-      </c>
-      <c r="C206" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3">
-      <c r="B207" t="s">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B207" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C207" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3">
-      <c r="B208" t="s">
+      <c r="C207" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B208" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C208" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3">
-      <c r="A210" t="s">
+      <c r="C208" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A210" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B210" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C210" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
-      <c r="A212" t="s">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A212" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B212" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C212" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="214" spans="1:3">
-      <c r="A214" t="s">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A214" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B214" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C214" t="s">
+      <c r="C214" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="215" spans="1:3">
-      <c r="B215" t="s">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B215" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C215" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="216" spans="1:3">
-      <c r="B216" t="s">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B216" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C216" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
-      <c r="B217" t="s">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B217" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C217" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="219" spans="1:3">
-      <c r="A219" t="s">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A219" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B219" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C219" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="220" spans="1:3">
-      <c r="B220" t="s">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B220" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C220" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="222" spans="1:3">
-      <c r="A222" t="s">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A222" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B222" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C222" t="s">
+      <c r="C222" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="223" spans="1:3">
-      <c r="B223" t="s">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B223" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C223" t="s">
+      <c r="C223" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="225" spans="1:3">
-      <c r="A225" t="s">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A225" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B225" t="s">
+      <c r="B225" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C225" t="s">
+      <c r="C225" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="226" spans="1:3">
-      <c r="B226" t="s">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B226" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C226" t="s">
+      <c r="C226" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="227" spans="1:3">
-      <c r="B227" t="s">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B227" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C227" t="s">
+      <c r="C227" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="228" spans="1:3">
-      <c r="B228" t="s">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B228" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C228" t="s">
+      <c r="C228" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="229" spans="1:3">
-      <c r="B229" t="s">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B229" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C229" t="s">
+      <c r="C229" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="230" spans="1:3">
-      <c r="B230" t="s">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B230" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C230" t="s">
+      <c r="C230" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="231" spans="1:3">
-      <c r="C231" t="s">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="C231" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="232" spans="1:3">
-      <c r="A232" t="s">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A232" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B232" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C232" t="s">
+      <c r="C232" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="233" spans="1:3">
-      <c r="B233" t="s">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B233" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C233" t="s">
+      <c r="C233" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="234" spans="1:3">
-      <c r="B234" t="s">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B234" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C234" t="s">
+      <c r="C234" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="236" spans="1:3">
-      <c r="A236" t="s">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A236" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B236" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C236" t="s">
+      <c r="C236" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="237" spans="1:3">
-      <c r="B237" t="s">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B237" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C237" t="s">
+      <c r="C237" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="238" spans="1:3">
-      <c r="B238" t="s">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B238" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C238" t="s">
+      <c r="C238" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="239" spans="1:3">
-      <c r="B239" t="s">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B239" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C239" t="s">
+      <c r="C239" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="240" spans="1:3">
-      <c r="B240" t="s">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B240" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C240" t="s">
+      <c r="C240" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
-      <c r="B241" t="s">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B241" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C241" t="s">
+      <c r="C241" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
-      <c r="B242" t="s">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B242" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C242" t="s">
+      <c r="C242" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="243" spans="1:3">
-      <c r="B243" t="s">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B243" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C243" t="s">
+      <c r="C243" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
-      <c r="B244" t="s">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B244" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C244" t="s">
+      <c r="C244" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
-      <c r="B245" t="s">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B245" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C245" t="s">
+      <c r="C245" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="247" spans="1:3">
-      <c r="A247" t="s">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A247" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B247" t="s">
+      <c r="B247" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C247" t="s">
+      <c r="C247" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="248" spans="1:3">
-      <c r="B248" t="s">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B248" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C248" t="s">
+      <c r="C248" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="249" spans="1:3">
-      <c r="B249" t="s">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B249" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C249" t="s">
+      <c r="C249" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="250" spans="1:3">
-      <c r="C250" t="s">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A251" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C251" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="251" spans="1:3">
-      <c r="A251" t="s">
-        <v>246</v>
-      </c>
-      <c r="B251" t="s">
-        <v>247</v>
-      </c>
-      <c r="C251" t="s">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B252" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C252" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="252" spans="1:3">
-      <c r="B252" t="s">
-        <v>248</v>
-      </c>
-      <c r="C252" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3">
-      <c r="B253" t="s">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B253" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C253" t="s">
+      <c r="C253" s="2" t="s">
         <v>206</v>
       </c>
     </row>

</xml_diff>